<commit_message>
SapCoExcelAddin: Add Activity Allocation Posting
</commit_message>
<xml_diff>
--- a/SAP_COOM_Planning_Total_V19.xlsx
+++ b/SAP_COOM_Planning_Total_V19.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS_WS\SapCoExcelAddin\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="360" windowWidth="11760" windowHeight="2475" tabRatio="328" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="360" windowWidth="11760" windowHeight="2475" tabRatio="407"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="4" r:id="rId1"/>
@@ -75,9 +75,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="132">
   <si>
-    <t>Paramter</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -469,6 +466,9 @@
   </si>
   <si>
     <t>600080</t>
+  </si>
+  <si>
+    <t>SAPCoOmPlanningTotal</t>
   </si>
 </sst>
 </file>
@@ -1436,8 +1436,8 @@
   <sheetPr codeName="Tabelle4"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1450,101 +1450,101 @@
   <sheetData>
     <row r="1" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="11">
         <v>2017</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="12">
         <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="11">
         <v>0</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="11">
         <v>0</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="37">
         <v>1798</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1589,55 +1589,55 @@
   <sheetData>
     <row r="1" spans="1:19" s="36" customFormat="1" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="39" t="s">
-        <v>10</v>
-      </c>
       <c r="C1" s="40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="44" t="s">
+      <c r="H1" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="I1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="J1" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="K1" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="46" t="s">
+      <c r="L1" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="M1" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="N1" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="44" t="s">
-        <v>33</v>
-      </c>
       <c r="O1" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="39" t="s">
-        <v>44</v>
-      </c>
       <c r="Q1" s="59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -1648,16 +1648,16 @@
         <v>303</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" s="63">
         <v>5696969.5099999998</v>
       </c>
       <c r="F2" s="64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G2" s="65">
         <v>0</v>
@@ -1705,16 +1705,16 @@
         <v>303</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" s="49">
         <v>12</v>
       </c>
       <c r="F3" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G3" s="51">
         <v>0</v>
@@ -1761,16 +1761,16 @@
         <v>303</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="49">
         <v>12</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G4" s="51">
         <v>0</v>
@@ -1817,16 +1817,16 @@
         <v>303</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="49">
         <v>12</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G5" s="51">
         <v>0</v>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B6" s="48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1883,7 +1883,7 @@
   <sheetPr codeName="Tabelle5"/>
   <dimension ref="A1:O249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1911,46 +1911,46 @@
   <sheetData>
     <row r="1" spans="1:15" s="36" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="D1" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="46" t="s">
+      <c r="G1" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="H1" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="I1" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="54" t="s">
-        <v>24</v>
-      </c>
       <c r="J1" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="L1" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="53" t="s">
+      <c r="M1" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="54" t="s">
-        <v>42</v>
-      </c>
       <c r="N1" s="54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -1958,10 +1958,10 @@
         <v>73000</v>
       </c>
       <c r="D2" s="48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E2" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F2" s="51">
         <v>-53569346.270000003</v>
@@ -1976,10 +1976,10 @@
         <v>70700</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E3" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F3" s="51">
         <v>-17561173</v>
@@ -1994,10 +1994,10 @@
         <v>73000</v>
       </c>
       <c r="D4" s="48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F4" s="51">
         <v>-9820937.1400000006</v>
@@ -2015,7 +2015,7 @@
         <v>760400</v>
       </c>
       <c r="E5" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F5" s="51">
         <v>-5850000</v>
@@ -2033,7 +2033,7 @@
         <v>500040</v>
       </c>
       <c r="E6" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F6" s="51">
         <v>-4687095</v>
@@ -2048,10 +2048,10 @@
         <v>73000</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E7" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F7" s="51">
         <v>-4687095</v>
@@ -2066,10 +2066,10 @@
         <v>73000</v>
       </c>
       <c r="D8" s="48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E8" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F8" s="51">
         <v>-579410</v>
@@ -2084,10 +2084,10 @@
         <v>70500</v>
       </c>
       <c r="D9" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E9" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F9" s="51">
         <v>800</v>
@@ -2102,10 +2102,10 @@
         <v>70600</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E10" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F10" s="51">
         <v>815.48</v>
@@ -2120,10 +2120,10 @@
         <v>70600</v>
       </c>
       <c r="D11" s="48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E11" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F11" s="51">
         <v>1000</v>
@@ -2138,10 +2138,10 @@
         <v>70200</v>
       </c>
       <c r="D12" s="48" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E12" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F12" s="51">
         <v>1000</v>
@@ -2156,10 +2156,10 @@
         <v>70700</v>
       </c>
       <c r="D13" s="48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E13" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F13" s="51">
         <v>2000</v>
@@ -2174,10 +2174,10 @@
         <v>70300</v>
       </c>
       <c r="D14" s="48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E14" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F14" s="51">
         <v>2000</v>
@@ -2192,10 +2192,10 @@
         <v>70600</v>
       </c>
       <c r="D15" s="48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E15" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F15" s="51">
         <v>2000</v>
@@ -2210,10 +2210,10 @@
         <v>70600</v>
       </c>
       <c r="D16" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E16" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F16" s="51">
         <v>2600</v>
@@ -2228,10 +2228,10 @@
         <v>70800</v>
       </c>
       <c r="D17" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E17" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F17" s="51">
         <v>3000</v>
@@ -2246,10 +2246,10 @@
         <v>73000</v>
       </c>
       <c r="D18" s="48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E18" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F18" s="51">
         <v>5000</v>
@@ -2264,10 +2264,10 @@
         <v>73000</v>
       </c>
       <c r="D19" s="48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E19" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F19" s="51">
         <v>5000</v>
@@ -2282,10 +2282,10 @@
         <v>73000</v>
       </c>
       <c r="D20" s="48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E20" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F20" s="51">
         <v>5000</v>
@@ -2300,10 +2300,10 @@
         <v>70700</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E21" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F21" s="51">
         <v>5000</v>
@@ -2318,10 +2318,10 @@
         <v>70400</v>
       </c>
       <c r="D22" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E22" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F22" s="51">
         <v>5000</v>
@@ -2336,10 +2336,10 @@
         <v>70400</v>
       </c>
       <c r="D23" s="48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E23" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F23" s="51">
         <v>5000</v>
@@ -2354,10 +2354,10 @@
         <v>73000</v>
       </c>
       <c r="D24" s="48" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E24" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F24" s="51">
         <v>5000</v>
@@ -2372,10 +2372,10 @@
         <v>70500</v>
       </c>
       <c r="D25" s="48" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E25" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F25" s="51">
         <v>6000</v>
@@ -2390,10 +2390,10 @@
         <v>70500</v>
       </c>
       <c r="D26" s="48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E26" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F26" s="51">
         <v>6000</v>
@@ -2408,10 +2408,10 @@
         <v>70800</v>
       </c>
       <c r="D27" s="48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E27" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F27" s="51">
         <v>6500</v>
@@ -2426,10 +2426,10 @@
         <v>70500</v>
       </c>
       <c r="D28" s="48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E28" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F28" s="51">
         <v>7000</v>
@@ -2444,10 +2444,10 @@
         <v>70100</v>
       </c>
       <c r="D29" s="48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E29" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F29" s="51">
         <v>7500</v>
@@ -2462,10 +2462,10 @@
         <v>70300</v>
       </c>
       <c r="D30" s="48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E30" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F30" s="51">
         <v>8000</v>
@@ -2480,10 +2480,10 @@
         <v>70200</v>
       </c>
       <c r="D31" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E31" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F31" s="51">
         <v>9000</v>
@@ -2498,10 +2498,10 @@
         <v>70600</v>
       </c>
       <c r="D32" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E32" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F32" s="51">
         <v>9000</v>
@@ -2516,10 +2516,10 @@
         <v>73000</v>
       </c>
       <c r="D33" s="48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E33" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F33" s="51">
         <v>10000</v>
@@ -2534,10 +2534,10 @@
         <v>70600</v>
       </c>
       <c r="D34" s="48" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E34" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F34" s="51">
         <v>10000</v>
@@ -2552,10 +2552,10 @@
         <v>70700</v>
       </c>
       <c r="D35" s="48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E35" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F35" s="51">
         <v>10000</v>
@@ -2570,10 +2570,10 @@
         <v>79200</v>
       </c>
       <c r="D36" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E36" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F36" s="51">
         <v>10000</v>
@@ -2588,10 +2588,10 @@
         <v>79200</v>
       </c>
       <c r="D37" s="48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E37" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F37" s="51">
         <v>10000</v>
@@ -2609,7 +2609,7 @@
         <v>632445</v>
       </c>
       <c r="E38" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F38" s="51">
         <v>10107.76</v>
@@ -2627,7 +2627,7 @@
         <v>632445</v>
       </c>
       <c r="E39" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F39" s="51">
         <v>10738</v>
@@ -2642,10 +2642,10 @@
         <v>76310</v>
       </c>
       <c r="D40" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E40" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F40" s="51">
         <v>11146.72</v>
@@ -2660,10 +2660,10 @@
         <v>70400</v>
       </c>
       <c r="D41" s="48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E41" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F41" s="51">
         <v>12000</v>
@@ -2681,7 +2681,7 @@
         <v>632445</v>
       </c>
       <c r="E42" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F42" s="51">
         <v>12299.04</v>
@@ -2696,10 +2696,10 @@
         <v>75100</v>
       </c>
       <c r="D43" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E43" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F43" s="51">
         <v>12752.48</v>
@@ -2714,10 +2714,10 @@
         <v>70800</v>
       </c>
       <c r="D44" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E44" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F44" s="51">
         <v>13500</v>
@@ -2732,10 +2732,10 @@
         <v>70500</v>
       </c>
       <c r="D45" s="48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E45" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F45" s="51">
         <v>14000</v>
@@ -2750,10 +2750,10 @@
         <v>74800</v>
       </c>
       <c r="D46" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E46" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F46" s="51">
         <v>14000.48</v>
@@ -2771,7 +2771,7 @@
         <v>632445</v>
       </c>
       <c r="E47" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F47" s="51">
         <v>14341.6</v>
@@ -2786,10 +2786,10 @@
         <v>70500</v>
       </c>
       <c r="D48" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E48" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F48" s="51">
         <v>14800</v>
@@ -2804,10 +2804,10 @@
         <v>73000</v>
       </c>
       <c r="D49" s="48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E49" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F49" s="51">
         <v>15000</v>
@@ -2822,10 +2822,10 @@
         <v>70700</v>
       </c>
       <c r="D50" s="48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E50" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F50" s="51">
         <v>15000</v>
@@ -2840,10 +2840,10 @@
         <v>73000</v>
       </c>
       <c r="D51" s="48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E51" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F51" s="51">
         <v>15000</v>
@@ -2858,10 +2858,10 @@
         <v>70700</v>
       </c>
       <c r="D52" s="48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E52" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F52" s="51">
         <v>15000</v>
@@ -2876,10 +2876,10 @@
         <v>70200</v>
       </c>
       <c r="D53" s="48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E53" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F53" s="51">
         <v>15000</v>
@@ -2894,10 +2894,10 @@
         <v>79200</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E54" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F54" s="51">
         <v>15000</v>
@@ -2912,10 +2912,10 @@
         <v>70800</v>
       </c>
       <c r="D55" s="48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E55" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F55" s="51">
         <v>15000</v>
@@ -2930,10 +2930,10 @@
         <v>70600</v>
       </c>
       <c r="D56" s="48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E56" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F56" s="51">
         <v>15000</v>
@@ -2948,10 +2948,10 @@
         <v>74120</v>
       </c>
       <c r="D57" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E57" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F57" s="51">
         <v>19811.61</v>
@@ -2966,10 +2966,10 @@
         <v>70200</v>
       </c>
       <c r="D58" s="48" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E58" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F58" s="51">
         <v>20500</v>
@@ -2984,10 +2984,10 @@
         <v>70300</v>
       </c>
       <c r="D59" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E59" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F59" s="51">
         <v>22000</v>
@@ -3002,10 +3002,10 @@
         <v>70600</v>
       </c>
       <c r="D60" s="48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E60" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F60" s="51">
         <v>23000</v>
@@ -3020,10 +3020,10 @@
         <v>70400</v>
       </c>
       <c r="D61" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E61" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F61" s="51">
         <v>23243.279999999999</v>
@@ -3038,10 +3038,10 @@
         <v>70150</v>
       </c>
       <c r="D62" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E62" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F62" s="51">
         <v>24000</v>
@@ -3056,10 +3056,10 @@
         <v>74300</v>
       </c>
       <c r="D63" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E63" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F63" s="51">
         <v>24660.48</v>
@@ -3074,10 +3074,10 @@
         <v>70700</v>
       </c>
       <c r="D64" s="48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E64" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F64" s="51">
         <v>25000</v>
@@ -3092,10 +3092,10 @@
         <v>70100</v>
       </c>
       <c r="D65" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E65" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F65" s="51">
         <v>25000</v>
@@ -3110,10 +3110,10 @@
         <v>79200</v>
       </c>
       <c r="D66" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E66" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F66" s="51">
         <v>25000</v>
@@ -3128,10 +3128,10 @@
         <v>73000</v>
       </c>
       <c r="D67" s="48" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E67" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F67" s="51">
         <v>25000</v>
@@ -3146,10 +3146,10 @@
         <v>80100</v>
       </c>
       <c r="D68" s="48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E68" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F68" s="51">
         <v>25000</v>
@@ -3164,10 +3164,10 @@
         <v>70700</v>
       </c>
       <c r="D69" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E69" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F69" s="51">
         <v>25000</v>
@@ -3185,7 +3185,7 @@
         <v>632445</v>
       </c>
       <c r="E70" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F70" s="51">
         <v>25967.759999999998</v>
@@ -3200,10 +3200,10 @@
         <v>70400</v>
       </c>
       <c r="D71" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E71" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F71" s="51">
         <v>26000</v>
@@ -3218,10 +3218,10 @@
         <v>79200</v>
       </c>
       <c r="D72" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E72" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F72" s="51">
         <v>26460.25</v>
@@ -3236,10 +3236,10 @@
         <v>70400</v>
       </c>
       <c r="D73" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E73" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F73" s="51">
         <v>26678.080000000002</v>
@@ -3254,10 +3254,10 @@
         <v>70600</v>
       </c>
       <c r="D74" s="48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E74" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F74" s="51">
         <v>30000</v>
@@ -3272,10 +3272,10 @@
         <v>80100</v>
       </c>
       <c r="D75" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E75" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F75" s="51">
         <v>30000</v>
@@ -3290,10 +3290,10 @@
         <v>75100</v>
       </c>
       <c r="D76" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E76" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F76" s="51">
         <v>30412.98</v>
@@ -3308,10 +3308,10 @@
         <v>70150</v>
       </c>
       <c r="D77" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E77" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F77" s="51">
         <v>31500</v>
@@ -3326,10 +3326,10 @@
         <v>70400</v>
       </c>
       <c r="D78" s="48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E78" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F78" s="51">
         <v>34000</v>
@@ -3344,10 +3344,10 @@
         <v>70150</v>
       </c>
       <c r="D79" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E79" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F79" s="51">
         <v>34812.36</v>
@@ -3362,10 +3362,10 @@
         <v>73000</v>
       </c>
       <c r="D80" s="48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E80" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F80" s="51">
         <v>35000</v>
@@ -3380,10 +3380,10 @@
         <v>70300</v>
       </c>
       <c r="D81" s="48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E81" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F81" s="51">
         <v>35000</v>
@@ -3398,10 +3398,10 @@
         <v>70150</v>
       </c>
       <c r="D82" s="48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E82" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F82" s="51">
         <v>35000</v>
@@ -3416,10 +3416,10 @@
         <v>80100</v>
       </c>
       <c r="D83" s="48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E83" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F83" s="51">
         <v>35000</v>
@@ -3437,7 +3437,7 @@
         <v>632445</v>
       </c>
       <c r="E84" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F84" s="51">
         <v>35551.360000000001</v>
@@ -3452,10 +3452,10 @@
         <v>70500</v>
       </c>
       <c r="D85" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E85" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F85" s="51">
         <v>36423.919999999998</v>
@@ -3473,7 +3473,7 @@
         <v>632445</v>
       </c>
       <c r="E86" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F86" s="51">
         <v>36579.919999999998</v>
@@ -3488,10 +3488,10 @@
         <v>74300</v>
       </c>
       <c r="D87" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E87" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F87" s="51">
         <v>38282.400000000001</v>
@@ -3506,10 +3506,10 @@
         <v>70700</v>
       </c>
       <c r="D88" s="48" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E88" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F88" s="51">
         <v>40000</v>
@@ -3527,7 +3527,7 @@
         <v>694160</v>
       </c>
       <c r="E89" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F89" s="51">
         <v>40000</v>
@@ -3542,10 +3542,10 @@
         <v>70700</v>
       </c>
       <c r="D90" s="48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E90" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F90" s="51">
         <v>40000</v>
@@ -3560,10 +3560,10 @@
         <v>70700</v>
       </c>
       <c r="D91" s="48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E91" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F91" s="51">
         <v>40000</v>
@@ -3578,10 +3578,10 @@
         <v>74120</v>
       </c>
       <c r="D92" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E92" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F92" s="51">
         <v>44025.8</v>
@@ -3596,10 +3596,10 @@
         <v>70600</v>
       </c>
       <c r="D93" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E93" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F93" s="51">
         <v>44815.71</v>
@@ -3614,10 +3614,10 @@
         <v>70100</v>
       </c>
       <c r="D94" s="48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E94" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F94" s="51">
         <v>45000</v>
@@ -3632,10 +3632,10 @@
         <v>70700</v>
       </c>
       <c r="D95" s="48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E95" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F95" s="51">
         <v>45000</v>
@@ -3650,10 +3650,10 @@
         <v>70100</v>
       </c>
       <c r="D96" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E96" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F96" s="51">
         <v>45000</v>
@@ -3668,10 +3668,10 @@
         <v>78100</v>
       </c>
       <c r="D97" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E97" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F97" s="51">
         <v>45260.800000000003</v>
@@ -3686,10 +3686,10 @@
         <v>70500</v>
       </c>
       <c r="D98" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E98" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F98" s="51">
         <v>45779.8</v>
@@ -3704,10 +3704,10 @@
         <v>70800</v>
       </c>
       <c r="D99" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E99" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F99" s="51">
         <v>46075.19</v>
@@ -3722,10 +3722,10 @@
         <v>70200</v>
       </c>
       <c r="D100" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E100" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F100" s="51">
         <v>49000</v>
@@ -3740,10 +3740,10 @@
         <v>74200</v>
       </c>
       <c r="D101" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E101" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F101" s="51">
         <v>49115.040000000001</v>
@@ -3761,7 +3761,7 @@
         <v>632445</v>
       </c>
       <c r="E102" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F102" s="51">
         <v>49541.64</v>
@@ -3776,10 +3776,10 @@
         <v>73000</v>
       </c>
       <c r="D103" s="48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E103" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F103" s="51">
         <v>50000</v>
@@ -3794,10 +3794,10 @@
         <v>73000</v>
       </c>
       <c r="D104" s="48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E104" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F104" s="51">
         <v>50000</v>
@@ -3812,10 +3812,10 @@
         <v>70300</v>
       </c>
       <c r="D105" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E105" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F105" s="51">
         <v>50000</v>
@@ -3830,10 +3830,10 @@
         <v>70700</v>
       </c>
       <c r="D106" s="48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E106" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F106" s="51">
         <v>50000</v>
@@ -3851,7 +3851,7 @@
         <v>632445</v>
       </c>
       <c r="E107" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F107" s="51">
         <v>50434.8</v>
@@ -3866,10 +3866,10 @@
         <v>70800</v>
       </c>
       <c r="D108" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E108" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F108" s="51">
         <v>52346.32</v>
@@ -3884,10 +3884,10 @@
         <v>70600</v>
       </c>
       <c r="D109" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E109" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F109" s="51">
         <v>53328.08</v>
@@ -3902,10 +3902,10 @@
         <v>70400</v>
       </c>
       <c r="D110" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E110" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F110" s="51">
         <v>54690.06</v>
@@ -3920,10 +3920,10 @@
         <v>73000</v>
       </c>
       <c r="D111" s="48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E111" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F111" s="51">
         <v>55000</v>
@@ -3938,10 +3938,10 @@
         <v>70150</v>
       </c>
       <c r="D112" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E112" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F112" s="51">
         <v>55546.400000000001</v>
@@ -3959,7 +3959,7 @@
         <v>632445</v>
       </c>
       <c r="E113" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F113" s="51">
         <v>56472</v>
@@ -3974,10 +3974,10 @@
         <v>75200</v>
       </c>
       <c r="D114" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E114" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F114" s="51">
         <v>58606.080000000002</v>
@@ -3992,10 +3992,10 @@
         <v>79200</v>
       </c>
       <c r="D115" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E115" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F115" s="51">
         <v>58800.56</v>
@@ -4013,7 +4013,7 @@
         <v>632445</v>
       </c>
       <c r="E116" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F116" s="51">
         <v>58927.44</v>
@@ -4028,10 +4028,10 @@
         <v>79200</v>
       </c>
       <c r="D117" s="48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E117" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F117" s="51">
         <v>60000</v>
@@ -4046,10 +4046,10 @@
         <v>74800</v>
       </c>
       <c r="D118" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E118" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F118" s="51">
         <v>60825.96</v>
@@ -4064,10 +4064,10 @@
         <v>70700</v>
       </c>
       <c r="D119" s="48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E119" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F119" s="51">
         <v>65000</v>
@@ -4082,10 +4082,10 @@
         <v>78100</v>
       </c>
       <c r="D120" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E120" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F120" s="51">
         <v>67330.69</v>
@@ -4100,10 +4100,10 @@
         <v>75100</v>
       </c>
       <c r="D121" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E121" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F121" s="51">
         <v>67584.399999999994</v>
@@ -4121,7 +4121,7 @@
         <v>632445</v>
       </c>
       <c r="E122" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F122" s="51">
         <v>68346.720000000001</v>
@@ -4139,7 +4139,7 @@
         <v>632445</v>
       </c>
       <c r="E123" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F123" s="51">
         <v>70748.08</v>
@@ -4157,7 +4157,7 @@
         <v>632445</v>
       </c>
       <c r="E124" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F124" s="51">
         <v>74507.679999999993</v>
@@ -4172,10 +4172,10 @@
         <v>70100</v>
       </c>
       <c r="D125" s="48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E125" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F125" s="51">
         <v>75000</v>
@@ -4190,10 +4190,10 @@
         <v>76310</v>
       </c>
       <c r="D126" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E126" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F126" s="51">
         <v>76489.919999999998</v>
@@ -4208,10 +4208,10 @@
         <v>70600</v>
       </c>
       <c r="D127" s="48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E127" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F127" s="51">
         <v>80000</v>
@@ -4226,10 +4226,10 @@
         <v>70150</v>
       </c>
       <c r="D128" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E128" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F128" s="51">
         <v>81911.44</v>
@@ -4247,7 +4247,7 @@
         <v>632445</v>
       </c>
       <c r="E129" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F129" s="51">
         <v>82852.639999999999</v>
@@ -4262,10 +4262,10 @@
         <v>70200</v>
       </c>
       <c r="D130" s="48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E130" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F130" s="51">
         <v>84280</v>
@@ -4280,10 +4280,10 @@
         <v>76150</v>
       </c>
       <c r="D131" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E131" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F131" s="51">
         <v>85074.08</v>
@@ -4298,10 +4298,10 @@
         <v>76310</v>
       </c>
       <c r="D132" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E132" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F132" s="51">
         <v>92223.039999999994</v>
@@ -4316,10 +4316,10 @@
         <v>70700</v>
       </c>
       <c r="D133" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E133" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F133" s="51">
         <v>94551.54</v>
@@ -4334,10 +4334,10 @@
         <v>73000</v>
       </c>
       <c r="D134" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E134" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F134" s="51">
         <v>99696.58</v>
@@ -4352,10 +4352,10 @@
         <v>70700</v>
       </c>
       <c r="D135" s="48" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E135" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F135" s="51">
         <v>100000</v>
@@ -4370,10 +4370,10 @@
         <v>70600</v>
       </c>
       <c r="D136" s="48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E136" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F136" s="51">
         <v>100000</v>
@@ -4388,10 +4388,10 @@
         <v>70600</v>
       </c>
       <c r="D137" s="48" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E137" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F137" s="51">
         <v>100000</v>
@@ -4406,10 +4406,10 @@
         <v>73000</v>
       </c>
       <c r="D138" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E138" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F138" s="51">
         <v>101097.32</v>
@@ -4424,10 +4424,10 @@
         <v>74300</v>
       </c>
       <c r="D139" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E139" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F139" s="51">
         <v>102805.47</v>
@@ -4442,10 +4442,10 @@
         <v>70600</v>
       </c>
       <c r="D140" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E140" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F140" s="51">
         <v>105448.72</v>
@@ -4460,10 +4460,10 @@
         <v>70500</v>
       </c>
       <c r="D141" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E141" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F141" s="51">
         <v>107717.17</v>
@@ -4478,10 +4478,10 @@
         <v>70700</v>
       </c>
       <c r="D142" s="48" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E142" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F142" s="51">
         <v>108000</v>
@@ -4496,10 +4496,10 @@
         <v>70800</v>
       </c>
       <c r="D143" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E143" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F143" s="51">
         <v>108412.2</v>
@@ -4517,7 +4517,7 @@
         <v>632445</v>
       </c>
       <c r="E144" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F144" s="51">
         <v>111367.36</v>
@@ -4532,10 +4532,10 @@
         <v>70200</v>
       </c>
       <c r="D145" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E145" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F145" s="51">
         <v>112698.21</v>
@@ -4550,10 +4550,10 @@
         <v>70100</v>
       </c>
       <c r="D146" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E146" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F146" s="51">
         <v>113990.23</v>
@@ -4568,10 +4568,10 @@
         <v>77000</v>
       </c>
       <c r="D147" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E147" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F147" s="51">
         <v>118301.7</v>
@@ -4586,10 +4586,10 @@
         <v>70600</v>
       </c>
       <c r="D148" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E148" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F148" s="51">
         <v>120000</v>
@@ -4604,10 +4604,10 @@
         <v>73000</v>
       </c>
       <c r="D149" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E149" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F149" s="51">
         <v>120056.44</v>
@@ -4622,10 +4622,10 @@
         <v>70300</v>
       </c>
       <c r="D150" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E150" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F150" s="51">
         <v>121279.67</v>
@@ -4640,10 +4640,10 @@
         <v>76240</v>
       </c>
       <c r="D151" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E151" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F151" s="51">
         <v>125432.32000000001</v>
@@ -4658,10 +4658,10 @@
         <v>74800</v>
       </c>
       <c r="D152" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E152" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F152" s="51">
         <v>135168.79999999999</v>
@@ -4676,10 +4676,10 @@
         <v>73000</v>
       </c>
       <c r="D153" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E153" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F153" s="51">
         <v>140712</v>
@@ -4694,10 +4694,10 @@
         <v>76310</v>
       </c>
       <c r="D154" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E154" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F154" s="51">
         <v>147490.48000000001</v>
@@ -4712,10 +4712,10 @@
         <v>74300</v>
       </c>
       <c r="D155" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E155" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F155" s="51">
         <v>148848.99</v>
@@ -4730,10 +4730,10 @@
         <v>74200</v>
       </c>
       <c r="D156" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E156" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F156" s="51">
         <v>149499.46</v>
@@ -4748,10 +4748,10 @@
         <v>78100</v>
       </c>
       <c r="D157" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E157" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F157" s="51">
         <v>149623.76</v>
@@ -4766,10 +4766,10 @@
         <v>70300</v>
       </c>
       <c r="D158" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E158" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F158" s="51">
         <v>150000</v>
@@ -4784,10 +4784,10 @@
         <v>70200</v>
       </c>
       <c r="D159" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E159" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F159" s="51">
         <v>156421.20000000001</v>
@@ -4802,10 +4802,10 @@
         <v>70100</v>
       </c>
       <c r="D160" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E160" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F160" s="51">
         <v>164139.04</v>
@@ -4820,10 +4820,10 @@
         <v>73000</v>
       </c>
       <c r="D161" s="48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E161" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F161" s="51">
         <v>165000</v>
@@ -4838,10 +4838,10 @@
         <v>73000</v>
       </c>
       <c r="D162" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E162" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F162" s="51">
         <v>167095.5</v>
@@ -4856,10 +4856,10 @@
         <v>75200</v>
       </c>
       <c r="D163" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E163" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F163" s="51">
         <v>169326.42</v>
@@ -4874,10 +4874,10 @@
         <v>76150</v>
       </c>
       <c r="D164" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E164" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F164" s="51">
         <v>171795.92</v>
@@ -4892,10 +4892,10 @@
         <v>70500</v>
       </c>
       <c r="D165" s="48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E165" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F165" s="51">
         <v>200000</v>
@@ -4910,10 +4910,10 @@
         <v>70700</v>
       </c>
       <c r="D166" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E166" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F166" s="51">
         <v>200000</v>
@@ -4928,10 +4928,10 @@
         <v>73000</v>
       </c>
       <c r="D167" s="48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E167" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F167" s="51">
         <v>206325</v>
@@ -4946,10 +4946,10 @@
         <v>70700</v>
       </c>
       <c r="D168" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E168" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F168" s="51">
         <v>210000</v>
@@ -4964,10 +4964,10 @@
         <v>74120</v>
       </c>
       <c r="D169" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E169" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F169" s="51">
         <v>220129</v>
@@ -4982,10 +4982,10 @@
         <v>70700</v>
       </c>
       <c r="D170" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E170" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F170" s="51">
         <v>222474.2</v>
@@ -5000,10 +5000,10 @@
         <v>76310</v>
       </c>
       <c r="D171" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E171" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F171" s="51">
         <v>222542.42</v>
@@ -5018,10 +5018,10 @@
         <v>76310</v>
       </c>
       <c r="D172" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E172" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F172" s="51">
         <v>223425.07</v>
@@ -5036,10 +5036,10 @@
         <v>74300</v>
       </c>
       <c r="D173" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E173" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F173" s="51">
         <v>228456.59</v>
@@ -5054,10 +5054,10 @@
         <v>70700</v>
       </c>
       <c r="D174" s="48" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E174" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F174" s="51">
         <v>230000</v>
@@ -5072,10 +5072,10 @@
         <v>80100</v>
       </c>
       <c r="D175" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E175" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F175" s="51">
         <v>230538.06</v>
@@ -5090,10 +5090,10 @@
         <v>70500</v>
       </c>
       <c r="D176" s="48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E176" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F176" s="51">
         <v>250000</v>
@@ -5108,10 +5108,10 @@
         <v>73000</v>
       </c>
       <c r="D177" s="48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E177" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F177" s="51">
         <v>255000</v>
@@ -5126,10 +5126,10 @@
         <v>77000</v>
       </c>
       <c r="D178" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E178" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F178" s="51">
         <v>262892.65999999997</v>
@@ -5144,10 +5144,10 @@
         <v>80100</v>
       </c>
       <c r="D179" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E179" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F179" s="51">
         <v>265004.48</v>
@@ -5162,10 +5162,10 @@
         <v>70200</v>
       </c>
       <c r="D180" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E180" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F180" s="51">
         <v>265172.26</v>
@@ -5180,10 +5180,10 @@
         <v>70100</v>
       </c>
       <c r="D181" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E181" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F181" s="51">
         <v>268212.31</v>
@@ -5198,10 +5198,10 @@
         <v>70600</v>
       </c>
       <c r="D182" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E182" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F182" s="51">
         <v>270000</v>
@@ -5216,10 +5216,10 @@
         <v>70300</v>
       </c>
       <c r="D183" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E183" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F183" s="51">
         <v>270604.88</v>
@@ -5234,10 +5234,10 @@
         <v>70400</v>
       </c>
       <c r="D184" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E184" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F184" s="51">
         <v>273450.32</v>
@@ -5252,10 +5252,10 @@
         <v>70300</v>
       </c>
       <c r="D185" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E185" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F185" s="51">
         <v>285363.94</v>
@@ -5270,10 +5270,10 @@
         <v>79200</v>
       </c>
       <c r="D186" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E186" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F186" s="51">
         <v>294002.8</v>
@@ -5288,10 +5288,10 @@
         <v>73000</v>
       </c>
       <c r="D187" s="48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E187" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F187" s="51">
         <v>300000</v>
@@ -5306,10 +5306,10 @@
         <v>76240</v>
       </c>
       <c r="D188" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E188" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F188" s="51">
         <v>321184.09000000003</v>
@@ -5324,10 +5324,10 @@
         <v>70500</v>
       </c>
       <c r="D189" s="48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E189" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F189" s="51">
         <v>325000</v>
@@ -5342,10 +5342,10 @@
         <v>76310</v>
       </c>
       <c r="D190" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E190" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F190" s="51">
         <v>327756.62</v>
@@ -5360,10 +5360,10 @@
         <v>74300</v>
       </c>
       <c r="D191" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E191" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F191" s="51">
         <v>330775.53999999998</v>
@@ -5378,10 +5378,10 @@
         <v>74200</v>
       </c>
       <c r="D192" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E192" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F192" s="51">
         <v>332221.03000000003</v>
@@ -5396,10 +5396,10 @@
         <v>70700</v>
       </c>
       <c r="D193" s="48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E193" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F193" s="51">
         <v>332546.90000000002</v>
@@ -5414,10 +5414,10 @@
         <v>75100</v>
       </c>
       <c r="D194" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E194" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F194" s="51">
         <v>337922</v>
@@ -5432,10 +5432,10 @@
         <v>73000</v>
       </c>
       <c r="D195" s="48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E195" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F195" s="51">
         <v>339395</v>
@@ -5450,10 +5450,10 @@
         <v>70400</v>
       </c>
       <c r="D196" s="48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E196" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F196" s="51">
         <v>348300</v>
@@ -5468,10 +5468,10 @@
         <v>70300</v>
       </c>
       <c r="D197" s="48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E197" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F197" s="51">
         <v>350000</v>
@@ -5486,10 +5486,10 @@
         <v>70700</v>
       </c>
       <c r="D198" s="48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E198" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F198" s="51">
         <v>362577.6</v>
@@ -5504,10 +5504,10 @@
         <v>75200</v>
       </c>
       <c r="D199" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E199" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F199" s="51">
         <v>376280.94</v>
@@ -5522,10 +5522,10 @@
         <v>80100</v>
       </c>
       <c r="D200" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E200" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F200" s="51">
         <v>379282</v>
@@ -5540,10 +5540,10 @@
         <v>76150</v>
       </c>
       <c r="D201" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E201" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F201" s="51">
         <v>381768.71</v>
@@ -5558,10 +5558,10 @@
         <v>70150</v>
       </c>
       <c r="D202" s="48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E202" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F202" s="51">
         <v>400000</v>
@@ -5576,10 +5576,10 @@
         <v>70150</v>
       </c>
       <c r="D203" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E203" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F203" s="51">
         <v>409557.2</v>
@@ -5594,10 +5594,10 @@
         <v>76310</v>
       </c>
       <c r="D204" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E204" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F204" s="51">
         <v>494538.72</v>
@@ -5612,10 +5612,10 @@
         <v>76310</v>
       </c>
       <c r="D205" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E205" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F205" s="51">
         <v>496500.16</v>
@@ -5630,10 +5630,10 @@
         <v>73000</v>
       </c>
       <c r="D206" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E206" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F206" s="51">
         <v>498482.92</v>
@@ -5651,7 +5651,7 @@
         <v>0</v>
       </c>
       <c r="E207" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F207" s="51">
         <v>500000</v>
@@ -5666,10 +5666,10 @@
         <v>80100</v>
       </c>
       <c r="D208" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E208" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F208" s="51">
         <v>512306.81</v>
@@ -5684,10 +5684,10 @@
         <v>70600</v>
       </c>
       <c r="D209" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E209" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F209" s="51">
         <v>527243.6</v>
@@ -5702,10 +5702,10 @@
         <v>70500</v>
       </c>
       <c r="D210" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E210" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F210" s="51">
         <v>538585.84</v>
@@ -5720,10 +5720,10 @@
         <v>70800</v>
       </c>
       <c r="D211" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E211" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F211" s="51">
         <v>542061</v>
@@ -5738,10 +5738,10 @@
         <v>73000</v>
       </c>
       <c r="D212" s="48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E212" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F212" s="51">
         <v>650000</v>
@@ -5756,10 +5756,10 @@
         <v>74800</v>
       </c>
       <c r="D213" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E213" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F213" s="51">
         <v>675844</v>
@@ -5774,10 +5774,10 @@
         <v>73000</v>
       </c>
       <c r="D214" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E214" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F214" s="51">
         <v>692000</v>
@@ -5792,10 +5792,10 @@
         <v>76240</v>
       </c>
       <c r="D215" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E215" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F215" s="51">
         <v>713742.43</v>
@@ -5810,10 +5810,10 @@
         <v>78100</v>
       </c>
       <c r="D216" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E216" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F216" s="51">
         <v>748118.8</v>
@@ -5828,10 +5828,10 @@
         <v>73000</v>
       </c>
       <c r="D217" s="48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E217" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F217" s="51">
         <v>750000</v>
@@ -5846,10 +5846,10 @@
         <v>73000</v>
       </c>
       <c r="D218" s="48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E218" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F218" s="51">
         <v>759936</v>
@@ -5864,10 +5864,10 @@
         <v>73000</v>
       </c>
       <c r="D219" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E219" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F219" s="51">
         <v>810077</v>
@@ -5885,7 +5885,7 @@
         <v>630000</v>
       </c>
       <c r="E220" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F220" s="51">
         <v>835477.5</v>
@@ -5900,10 +5900,10 @@
         <v>73000</v>
       </c>
       <c r="D221" s="48" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E221" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F221" s="51">
         <v>950000</v>
@@ -5918,10 +5918,10 @@
         <v>70700</v>
       </c>
       <c r="D222" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E222" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F222" s="51">
         <v>1112371</v>
@@ -5936,10 +5936,10 @@
         <v>74300</v>
       </c>
       <c r="D223" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E223" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F223" s="51">
         <v>1142282.96</v>
@@ -5954,10 +5954,10 @@
         <v>70700</v>
       </c>
       <c r="D224" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E224" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F224" s="51">
         <v>1162804.56</v>
@@ -5972,10 +5972,10 @@
         <v>77000</v>
       </c>
       <c r="D225" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E225" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F225" s="51">
         <v>1314463.28</v>
@@ -5990,10 +5990,10 @@
         <v>70200</v>
       </c>
       <c r="D226" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E226" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F226" s="51">
         <v>1325861.28</v>
@@ -6008,10 +6008,10 @@
         <v>70100</v>
       </c>
       <c r="D227" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E227" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F227" s="51">
         <v>1341061.56</v>
@@ -6026,10 +6026,10 @@
         <v>70300</v>
       </c>
       <c r="D228" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E228" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F228" s="51">
         <v>1426819.68</v>
@@ -6044,10 +6044,10 @@
         <v>73000</v>
       </c>
       <c r="D229" s="48" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E229" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F229" s="51">
         <v>1457609</v>
@@ -6062,10 +6062,10 @@
         <v>73000</v>
       </c>
       <c r="D230" s="48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E230" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F230" s="51">
         <v>1621990</v>
@@ -6080,10 +6080,10 @@
         <v>76310</v>
       </c>
       <c r="D231" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E231" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F231" s="51">
         <v>1638783.12</v>
@@ -6098,10 +6098,10 @@
         <v>74300</v>
       </c>
       <c r="D232" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E232" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F232" s="51">
         <v>1653877.68</v>
@@ -6116,10 +6116,10 @@
         <v>74200</v>
       </c>
       <c r="D233" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E233" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F233" s="51">
         <v>1661105.16</v>
@@ -6134,10 +6134,10 @@
         <v>73000</v>
       </c>
       <c r="D234" s="48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E234" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F234" s="51">
         <v>1711000</v>
@@ -6152,10 +6152,10 @@
         <v>73000</v>
       </c>
       <c r="D235" s="48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E235" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F235" s="51">
         <v>1721811</v>
@@ -6170,10 +6170,10 @@
         <v>75200</v>
       </c>
       <c r="D236" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E236" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F236" s="51">
         <v>1881404.72</v>
@@ -6188,10 +6188,10 @@
         <v>76150</v>
       </c>
       <c r="D237" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E237" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F237" s="51">
         <v>1908843.56</v>
@@ -6206,10 +6206,10 @@
         <v>70700</v>
       </c>
       <c r="D238" s="48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E238" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F238" s="51">
         <v>2300000</v>
@@ -6224,10 +6224,10 @@
         <v>76310</v>
       </c>
       <c r="D239" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E239" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F239" s="51">
         <v>2472693.6</v>
@@ -6242,10 +6242,10 @@
         <v>76310</v>
       </c>
       <c r="D240" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E240" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F240" s="51">
         <v>2482500.7999999998</v>
@@ -6260,10 +6260,10 @@
         <v>80100</v>
       </c>
       <c r="D241" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E241" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F241" s="51">
         <v>2561534.04</v>
@@ -6278,10 +6278,10 @@
         <v>73000</v>
       </c>
       <c r="D242" s="48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E242" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F242" s="51">
         <v>2877879</v>
@@ -6296,10 +6296,10 @@
         <v>73000</v>
       </c>
       <c r="D243" s="48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E243" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F243" s="51">
         <v>3545645</v>
@@ -6314,10 +6314,10 @@
         <v>76240</v>
       </c>
       <c r="D244" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E244" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F244" s="51">
         <v>3568712.16</v>
@@ -6332,10 +6332,10 @@
         <v>73000</v>
       </c>
       <c r="D245" s="48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E245" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F245" s="51">
         <v>3655260</v>
@@ -6350,10 +6350,10 @@
         <v>73000</v>
       </c>
       <c r="D246" s="48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E246" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F246" s="51">
         <v>4083192.86</v>
@@ -6368,10 +6368,10 @@
         <v>73000</v>
       </c>
       <c r="D247" s="48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E247" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F247" s="51">
         <v>4687095</v>
@@ -6386,10 +6386,10 @@
         <v>73000</v>
       </c>
       <c r="D248" s="48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E248" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F248" s="51">
         <v>10226675</v>
@@ -6438,34 +6438,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="36" customFormat="1" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" s="39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="41" t="s">
-        <v>16</v>
-      </c>
       <c r="G1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="I1" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="J1" s="45" t="s">
         <v>37</v>
-      </c>
-      <c r="J1" s="45" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -6499,55 +6499,55 @@
   <sheetData>
     <row r="1" spans="1:17" s="35" customFormat="1" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="F1" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="G1" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="I1" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="J1" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="K1" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="L1" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="M1" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="N1" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="32" t="s">
+      <c r="O1" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="O1" s="32" t="s">
+      <c r="P1" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="32" t="s">
+      <c r="Q1" s="33" t="s">
         <v>57</v>
-      </c>
-      <c r="Q1" s="33" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -6756,10 +6756,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6771,29 +6772,29 @@
   <sheetData>
     <row r="1" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" s="68"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="77">
         <v>0</v>
@@ -6801,67 +6802,67 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="16"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="16"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="16"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="69" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" s="71" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" s="73"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="74" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="75" t="s">
         <v>75</v>
-      </c>
-      <c r="B13" s="75" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="76" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="71" t="s">
         <v>77</v>
-      </c>
-      <c r="B14" s="71" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>